<commit_message>
penambahan file baru perbaikan
</commit_message>
<xml_diff>
--- a/Financial_report.xlsx
+++ b/Financial_report.xlsx
@@ -516,14 +516,14 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -849,40 +849,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F35"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1447,41 +1447,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="str">
+      <c r="B1" s="22" t="str">
         <f>Neraca!B1</f>
         <v>PT. SEPATU BATA Tbk.</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="8"/>
@@ -1746,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,12 +2115,12 @@
         <v>104</v>
       </c>
       <c r="E37" s="11">
-        <f>Laba_Rugi!E32</f>
-        <v>128895612</v>
+        <f>Laba_Rugi!E25</f>
+        <v>129519446</v>
       </c>
       <c r="F37" s="18">
         <f>E37/E38</f>
-        <v>0.16208025095514478</v>
+        <v>0.16286469326241551</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,11 +2147,11 @@
       </c>
       <c r="E40" s="11">
         <f>E37</f>
-        <v>128895612</v>
+        <v>129519446</v>
       </c>
       <c r="F40" s="18">
         <f>E40/E41</f>
-        <v>0.23556035323106456</v>
+        <v>0.23670042739741826</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,11 +2175,11 @@
       </c>
       <c r="E43" s="11">
         <f>E40</f>
-        <v>128895612</v>
+        <v>129519446</v>
       </c>
       <c r="F43" s="18">
         <f>E43/E44</f>
-        <v>0.12528117761333463</v>
+        <v>0.12588751833310435</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="F46" s="18">
         <f>F43*F25</f>
-        <v>0.16208025095514478</v>
+        <v>0.16286469326241551</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
       <c r="C48" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="20">
         <f>Neraca!E54</f>
         <v>248070766</v>
       </c>
@@ -2243,11 +2243,11 @@
       </c>
       <c r="E51" s="16">
         <f>F46</f>
-        <v>0.16208025095514478</v>
+        <v>0.16286469326241551</v>
       </c>
       <c r="F51" s="18">
         <f>(E51/E52)</f>
-        <v>0.23556035323106458</v>
+        <v>0.23670042739741828</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>